<commit_message>
ACET Maturity Results page
</commit_message>
<xml_diff>
--- a/CSETWebApi/CSETWeb_Api/CSETWebCore.Business/App_Data/Spanish ACET Groupings.xlsx
+++ b/CSETWebApi/CSETWeb_Api/CSETWebCore.Business/App_Data/Spanish ACET Groupings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inl-my.sharepoint.com/personal/matthew_winston_inl_gov/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WINSMR\cset\CSETWebApi\CSETWeb_Api\CSETWebCore.Business\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB9BE65D-A39F-4827-9AF2-54ACF998FCD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B10B546-D127-473E-B1D3-B13FB7FE3BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{262E682B-5CFD-4D9C-A77F-A2ABC044543A}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
   <si>
     <t>Grouping_Id</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>Sequence</t>
   </si>
   <si>
@@ -186,6 +183,150 @@
   </si>
   <si>
     <t>Proceso de Escalación y Registro</t>
+  </si>
+  <si>
+    <t>English_Title</t>
+  </si>
+  <si>
+    <t>Spanish_Title</t>
+  </si>
+  <si>
+    <t>Cyber Risk Management &amp; Oversight</t>
+  </si>
+  <si>
+    <t>Threat Intelligence &amp; Collaboration</t>
+  </si>
+  <si>
+    <t>Cybersecurity Controls</t>
+  </si>
+  <si>
+    <t>External Dependency Management</t>
+  </si>
+  <si>
+    <t>Cyber Incident Management and Resilience</t>
+  </si>
+  <si>
+    <t>Governance</t>
+  </si>
+  <si>
+    <t>Risk Management</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>Training and Culture</t>
+  </si>
+  <si>
+    <t>Threat Intelligence</t>
+  </si>
+  <si>
+    <t>Monitoring and Analyzing</t>
+  </si>
+  <si>
+    <t>Information Sharing</t>
+  </si>
+  <si>
+    <t>Preventative Controls</t>
+  </si>
+  <si>
+    <t>Detective Controls</t>
+  </si>
+  <si>
+    <t>Corrective Controls</t>
+  </si>
+  <si>
+    <t>Connections</t>
+  </si>
+  <si>
+    <t>Relationship Management</t>
+  </si>
+  <si>
+    <t>Incident Resilience Planning and Strategy</t>
+  </si>
+  <si>
+    <t>Detection, Response, and Mitigation</t>
+  </si>
+  <si>
+    <t>Escalation and Reporting</t>
+  </si>
+  <si>
+    <t>Oversight</t>
+  </si>
+  <si>
+    <t>Strategy / Policies</t>
+  </si>
+  <si>
+    <t>IT Asset Management</t>
+  </si>
+  <si>
+    <t>Risk Management Program</t>
+  </si>
+  <si>
+    <t>Risk Assessment</t>
+  </si>
+  <si>
+    <t>Audit</t>
+  </si>
+  <si>
+    <t>Staffing</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Culture</t>
+  </si>
+  <si>
+    <t>Threat Intelligence and Information</t>
+  </si>
+  <si>
+    <t>Infrastructure Management</t>
+  </si>
+  <si>
+    <t>Access and Data Management</t>
+  </si>
+  <si>
+    <t>Device / End-Point Security</t>
+  </si>
+  <si>
+    <t>Secure Coding</t>
+  </si>
+  <si>
+    <t>Threat and Vulnerability Detection</t>
+  </si>
+  <si>
+    <t>Anomalous Activity Detection</t>
+  </si>
+  <si>
+    <t>Event Detection</t>
+  </si>
+  <si>
+    <t>Patch Management</t>
+  </si>
+  <si>
+    <t>Remediation</t>
+  </si>
+  <si>
+    <t>Due Diligence</t>
+  </si>
+  <si>
+    <t>Contracts</t>
+  </si>
+  <si>
+    <t>Ongoing Monitoring</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Detection</t>
+  </si>
+  <si>
+    <t>Response and Mitigation</t>
   </si>
 </sst>
 </file>
@@ -537,729 +678,883 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C34376-EFFC-4E41-8D7B-99B9F2867C18}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="39.88671875" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="39.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>93</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
       </c>
       <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>94</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
         <v>3</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
         <v>4</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
       </c>
       <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>98</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12">
         <v>2</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13">
         <v>3</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
       </c>
       <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15">
         <v>2</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>102</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16">
         <v>3</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
       </c>
       <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>104</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18">
         <v>2</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>105</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
       </c>
       <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20">
         <v>2</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>107</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21">
         <v>3</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>108</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
       </c>
       <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>109</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23">
         <v>2</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24">
         <v>3</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
+        <v>74</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
       </c>
       <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>112</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26">
         <v>2</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27">
         <v>3</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>114</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
       </c>
       <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
       </c>
       <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30">
+        <v>79</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30">
         <v>2</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>117</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
       </c>
       <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>20</v>
       </c>
       <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
       </c>
       <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>120</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
+        <v>81</v>
+      </c>
+      <c r="C34" t="s">
+        <v>25</v>
       </c>
       <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>121</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35">
+        <v>82</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35">
         <v>2</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>122</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36">
+        <v>83</v>
+      </c>
+      <c r="C36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36">
         <v>3</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>123</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37">
+        <v>84</v>
+      </c>
+      <c r="C37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37">
         <v>4</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>124</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
+        <v>85</v>
+      </c>
+      <c r="C38" t="s">
+        <v>31</v>
       </c>
       <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>125</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39">
+        <v>86</v>
+      </c>
+      <c r="C39" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39">
         <v>2</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40">
+        <v>87</v>
+      </c>
+      <c r="C40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40">
         <v>3</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>127</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="C41" t="s">
+        <v>34</v>
       </c>
       <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>128</v>
       </c>
       <c r="B42" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42">
+        <v>89</v>
+      </c>
+      <c r="C42" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42">
         <v>2</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>129</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
       </c>
       <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>130</v>
       </c>
       <c r="B44" t="s">
-        <v>39</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="C44" t="s">
+        <v>38</v>
       </c>
       <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>131</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
-      </c>
-      <c r="C45">
+        <v>91</v>
+      </c>
+      <c r="C45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45">
         <v>2</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>132</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
-      </c>
-      <c r="C46">
+        <v>92</v>
+      </c>
+      <c r="C46" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46">
         <v>3</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>133</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="C47" t="s">
+        <v>42</v>
       </c>
       <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>134</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48">
+        <v>94</v>
+      </c>
+      <c r="C48" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48">
         <v>2</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>135</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
+        <v>95</v>
+      </c>
+      <c r="C49" t="s">
+        <v>45</v>
       </c>
       <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>136</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
-      </c>
-      <c r="C50">
+        <v>96</v>
+      </c>
+      <c r="C50" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50">
         <v>2</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>137</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="C51" t="s">
+        <v>48</v>
       </c>
       <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
         <v>107</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel typo fixes, irp summ. reloads on lang change
</commit_message>
<xml_diff>
--- a/CSETWebApi/CSETWeb_Api/CSETWebCore.Business/App_Data/Spanish ACET Groupings.xlsx
+++ b/CSETWebApi/CSETWeb_Api/CSETWebCore.Business/App_Data/Spanish ACET Groupings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WINSMR\cset\CSETWebApi\CSETWeb_Api\CSETWebCore.Business\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B10B546-D127-473E-B1D3-B13FB7FE3BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085C4788-67DB-4A13-BEA9-281DB793C184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{262E682B-5CFD-4D9C-A77F-A2ABC044543A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
   <si>
     <t>Grouping_Id</t>
   </si>
@@ -215,118 +215,121 @@
     <t>Resources</t>
   </si>
   <si>
-    <t>Training and Culture</t>
-  </si>
-  <si>
     <t>Threat Intelligence</t>
   </si>
   <si>
+    <t>Information Sharing</t>
+  </si>
+  <si>
+    <t>Preventative Controls</t>
+  </si>
+  <si>
+    <t>Detective Controls</t>
+  </si>
+  <si>
+    <t>Corrective Controls</t>
+  </si>
+  <si>
+    <t>Connections</t>
+  </si>
+  <si>
+    <t>Relationship Management</t>
+  </si>
+  <si>
+    <t>Incident Resilience Planning and Strategy</t>
+  </si>
+  <si>
+    <t>Detection, Response, and Mitigation</t>
+  </si>
+  <si>
+    <t>Escalation and Reporting</t>
+  </si>
+  <si>
+    <t>Oversight</t>
+  </si>
+  <si>
+    <t>Strategy / Policies</t>
+  </si>
+  <si>
+    <t>IT Asset Management</t>
+  </si>
+  <si>
+    <t>Risk Management Program</t>
+  </si>
+  <si>
+    <t>Risk Assessment</t>
+  </si>
+  <si>
+    <t>Audit</t>
+  </si>
+  <si>
+    <t>Staffing</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Culture</t>
+  </si>
+  <si>
+    <t>Threat Intelligence and Information</t>
+  </si>
+  <si>
+    <t>Infrastructure Management</t>
+  </si>
+  <si>
+    <t>Access and Data Management</t>
+  </si>
+  <si>
+    <t>Device / End-Point Security</t>
+  </si>
+  <si>
+    <t>Secure Coding</t>
+  </si>
+  <si>
+    <t>Threat and Vulnerability Detection</t>
+  </si>
+  <si>
+    <t>Anomalous Activity Detection</t>
+  </si>
+  <si>
+    <t>Event Detection</t>
+  </si>
+  <si>
+    <t>Patch Management</t>
+  </si>
+  <si>
+    <t>Remediation</t>
+  </si>
+  <si>
+    <t>Due Diligence</t>
+  </si>
+  <si>
+    <t>Contracts</t>
+  </si>
+  <si>
+    <t>Ongoing Monitoring</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Detection</t>
+  </si>
+  <si>
+    <t>Response and Mitigation</t>
+  </si>
+  <si>
+    <t>Training &amp; Culture</t>
+  </si>
+  <si>
+    <t>Monitoring &amp; Analyzing</t>
+  </si>
+  <si>
     <t>Monitoring and Analyzing</t>
-  </si>
-  <si>
-    <t>Information Sharing</t>
-  </si>
-  <si>
-    <t>Preventative Controls</t>
-  </si>
-  <si>
-    <t>Detective Controls</t>
-  </si>
-  <si>
-    <t>Corrective Controls</t>
-  </si>
-  <si>
-    <t>Connections</t>
-  </si>
-  <si>
-    <t>Relationship Management</t>
-  </si>
-  <si>
-    <t>Incident Resilience Planning and Strategy</t>
-  </si>
-  <si>
-    <t>Detection, Response, and Mitigation</t>
-  </si>
-  <si>
-    <t>Escalation and Reporting</t>
-  </si>
-  <si>
-    <t>Oversight</t>
-  </si>
-  <si>
-    <t>Strategy / Policies</t>
-  </si>
-  <si>
-    <t>IT Asset Management</t>
-  </si>
-  <si>
-    <t>Risk Management Program</t>
-  </si>
-  <si>
-    <t>Risk Assessment</t>
-  </si>
-  <si>
-    <t>Audit</t>
-  </si>
-  <si>
-    <t>Staffing</t>
-  </si>
-  <si>
-    <t>Training</t>
-  </si>
-  <si>
-    <t>Culture</t>
-  </si>
-  <si>
-    <t>Threat Intelligence and Information</t>
-  </si>
-  <si>
-    <t>Infrastructure Management</t>
-  </si>
-  <si>
-    <t>Access and Data Management</t>
-  </si>
-  <si>
-    <t>Device / End-Point Security</t>
-  </si>
-  <si>
-    <t>Secure Coding</t>
-  </si>
-  <si>
-    <t>Threat and Vulnerability Detection</t>
-  </si>
-  <si>
-    <t>Anomalous Activity Detection</t>
-  </si>
-  <si>
-    <t>Event Detection</t>
-  </si>
-  <si>
-    <t>Patch Management</t>
-  </si>
-  <si>
-    <t>Remediation</t>
-  </si>
-  <si>
-    <t>Due Diligence</t>
-  </si>
-  <si>
-    <t>Contracts</t>
-  </si>
-  <si>
-    <t>Ongoing Monitoring</t>
-  </si>
-  <si>
-    <t>Planning</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Detection</t>
-  </si>
-  <si>
-    <t>Response and Mitigation</t>
   </si>
 </sst>
 </file>
@@ -680,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C34376-EFFC-4E41-8D7B-99B9F2867C18}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,7 +852,7 @@
         <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -866,7 +869,7 @@
         <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
@@ -883,7 +886,7 @@
         <v>98</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
@@ -900,7 +903,7 @@
         <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
@@ -917,7 +920,7 @@
         <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -934,7 +937,7 @@
         <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
@@ -951,7 +954,7 @@
         <v>102</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
         <v>35</v>
@@ -968,7 +971,7 @@
         <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
         <v>37</v>
@@ -985,7 +988,7 @@
         <v>104</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
         <v>39</v>
@@ -1002,7 +1005,7 @@
         <v>105</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
         <v>43</v>
@@ -1019,7 +1022,7 @@
         <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
         <v>46</v>
@@ -1036,7 +1039,7 @@
         <v>107</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
         <v>48</v>
@@ -1053,7 +1056,7 @@
         <v>108</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -1070,7 +1073,7 @@
         <v>109</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -1087,7 +1090,7 @@
         <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -1104,7 +1107,7 @@
         <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
@@ -1121,7 +1124,7 @@
         <v>112</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -1138,7 +1141,7 @@
         <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
@@ -1155,7 +1158,7 @@
         <v>114</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
@@ -1172,7 +1175,7 @@
         <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
         <v>16</v>
@@ -1189,7 +1192,7 @@
         <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
@@ -1206,7 +1209,7 @@
         <v>117</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
@@ -1223,7 +1226,7 @@
         <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
         <v>20</v>
@@ -1240,7 +1243,7 @@
         <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
         <v>21</v>
@@ -1257,7 +1260,7 @@
         <v>120</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
         <v>25</v>
@@ -1274,7 +1277,7 @@
         <v>121</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C35" t="s">
         <v>27</v>
@@ -1291,7 +1294,7 @@
         <v>122</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C36" t="s">
         <v>28</v>
@@ -1308,7 +1311,7 @@
         <v>123</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C37" t="s">
         <v>29</v>
@@ -1325,7 +1328,7 @@
         <v>124</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C38" t="s">
         <v>31</v>
@@ -1342,7 +1345,7 @@
         <v>125</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C39" t="s">
         <v>32</v>
@@ -1359,7 +1362,7 @@
         <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C40" t="s">
         <v>33</v>
@@ -1376,7 +1379,7 @@
         <v>127</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C41" t="s">
         <v>34</v>
@@ -1393,7 +1396,7 @@
         <v>128</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
         <v>36</v>
@@ -1410,7 +1413,7 @@
         <v>129</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C43" t="s">
         <v>37</v>
@@ -1427,7 +1430,7 @@
         <v>130</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C44" t="s">
         <v>38</v>
@@ -1444,7 +1447,7 @@
         <v>131</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C45" t="s">
         <v>40</v>
@@ -1461,7 +1464,7 @@
         <v>132</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C46" t="s">
         <v>41</v>
@@ -1478,7 +1481,7 @@
         <v>133</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C47" t="s">
         <v>42</v>
@@ -1495,7 +1498,7 @@
         <v>134</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C48" t="s">
         <v>44</v>
@@ -1512,7 +1515,7 @@
         <v>135</v>
       </c>
       <c r="B49" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C49" t="s">
         <v>45</v>
@@ -1529,7 +1532,7 @@
         <v>136</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
         <v>47</v>
@@ -1546,7 +1549,7 @@
         <v>137</v>
       </c>
       <c r="B51" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C51" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
excel updates from develop
</commit_message>
<xml_diff>
--- a/CSETWebApi/CSETWeb_Api/CSETWebCore.Business/App_Data/Spanish ACET Groupings.xlsx
+++ b/CSETWebApi/CSETWeb_Api/CSETWebCore.Business/App_Data/Spanish ACET Groupings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WINSMR\cset\CSETWebApi\CSETWeb_Api\CSETWebCore.Business\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B10B546-D127-473E-B1D3-B13FB7FE3BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085C4788-67DB-4A13-BEA9-281DB793C184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{262E682B-5CFD-4D9C-A77F-A2ABC044543A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
   <si>
     <t>Grouping_Id</t>
   </si>
@@ -215,118 +215,121 @@
     <t>Resources</t>
   </si>
   <si>
-    <t>Training and Culture</t>
-  </si>
-  <si>
     <t>Threat Intelligence</t>
   </si>
   <si>
+    <t>Information Sharing</t>
+  </si>
+  <si>
+    <t>Preventative Controls</t>
+  </si>
+  <si>
+    <t>Detective Controls</t>
+  </si>
+  <si>
+    <t>Corrective Controls</t>
+  </si>
+  <si>
+    <t>Connections</t>
+  </si>
+  <si>
+    <t>Relationship Management</t>
+  </si>
+  <si>
+    <t>Incident Resilience Planning and Strategy</t>
+  </si>
+  <si>
+    <t>Detection, Response, and Mitigation</t>
+  </si>
+  <si>
+    <t>Escalation and Reporting</t>
+  </si>
+  <si>
+    <t>Oversight</t>
+  </si>
+  <si>
+    <t>Strategy / Policies</t>
+  </si>
+  <si>
+    <t>IT Asset Management</t>
+  </si>
+  <si>
+    <t>Risk Management Program</t>
+  </si>
+  <si>
+    <t>Risk Assessment</t>
+  </si>
+  <si>
+    <t>Audit</t>
+  </si>
+  <si>
+    <t>Staffing</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Culture</t>
+  </si>
+  <si>
+    <t>Threat Intelligence and Information</t>
+  </si>
+  <si>
+    <t>Infrastructure Management</t>
+  </si>
+  <si>
+    <t>Access and Data Management</t>
+  </si>
+  <si>
+    <t>Device / End-Point Security</t>
+  </si>
+  <si>
+    <t>Secure Coding</t>
+  </si>
+  <si>
+    <t>Threat and Vulnerability Detection</t>
+  </si>
+  <si>
+    <t>Anomalous Activity Detection</t>
+  </si>
+  <si>
+    <t>Event Detection</t>
+  </si>
+  <si>
+    <t>Patch Management</t>
+  </si>
+  <si>
+    <t>Remediation</t>
+  </si>
+  <si>
+    <t>Due Diligence</t>
+  </si>
+  <si>
+    <t>Contracts</t>
+  </si>
+  <si>
+    <t>Ongoing Monitoring</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Detection</t>
+  </si>
+  <si>
+    <t>Response and Mitigation</t>
+  </si>
+  <si>
+    <t>Training &amp; Culture</t>
+  </si>
+  <si>
+    <t>Monitoring &amp; Analyzing</t>
+  </si>
+  <si>
     <t>Monitoring and Analyzing</t>
-  </si>
-  <si>
-    <t>Information Sharing</t>
-  </si>
-  <si>
-    <t>Preventative Controls</t>
-  </si>
-  <si>
-    <t>Detective Controls</t>
-  </si>
-  <si>
-    <t>Corrective Controls</t>
-  </si>
-  <si>
-    <t>Connections</t>
-  </si>
-  <si>
-    <t>Relationship Management</t>
-  </si>
-  <si>
-    <t>Incident Resilience Planning and Strategy</t>
-  </si>
-  <si>
-    <t>Detection, Response, and Mitigation</t>
-  </si>
-  <si>
-    <t>Escalation and Reporting</t>
-  </si>
-  <si>
-    <t>Oversight</t>
-  </si>
-  <si>
-    <t>Strategy / Policies</t>
-  </si>
-  <si>
-    <t>IT Asset Management</t>
-  </si>
-  <si>
-    <t>Risk Management Program</t>
-  </si>
-  <si>
-    <t>Risk Assessment</t>
-  </si>
-  <si>
-    <t>Audit</t>
-  </si>
-  <si>
-    <t>Staffing</t>
-  </si>
-  <si>
-    <t>Training</t>
-  </si>
-  <si>
-    <t>Culture</t>
-  </si>
-  <si>
-    <t>Threat Intelligence and Information</t>
-  </si>
-  <si>
-    <t>Infrastructure Management</t>
-  </si>
-  <si>
-    <t>Access and Data Management</t>
-  </si>
-  <si>
-    <t>Device / End-Point Security</t>
-  </si>
-  <si>
-    <t>Secure Coding</t>
-  </si>
-  <si>
-    <t>Threat and Vulnerability Detection</t>
-  </si>
-  <si>
-    <t>Anomalous Activity Detection</t>
-  </si>
-  <si>
-    <t>Event Detection</t>
-  </si>
-  <si>
-    <t>Patch Management</t>
-  </si>
-  <si>
-    <t>Remediation</t>
-  </si>
-  <si>
-    <t>Due Diligence</t>
-  </si>
-  <si>
-    <t>Contracts</t>
-  </si>
-  <si>
-    <t>Ongoing Monitoring</t>
-  </si>
-  <si>
-    <t>Planning</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Detection</t>
-  </si>
-  <si>
-    <t>Response and Mitigation</t>
   </si>
 </sst>
 </file>
@@ -680,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C34376-EFFC-4E41-8D7B-99B9F2867C18}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,7 +852,7 @@
         <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -866,7 +869,7 @@
         <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
@@ -883,7 +886,7 @@
         <v>98</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
@@ -900,7 +903,7 @@
         <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
@@ -917,7 +920,7 @@
         <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -934,7 +937,7 @@
         <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
@@ -951,7 +954,7 @@
         <v>102</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
         <v>35</v>
@@ -968,7 +971,7 @@
         <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
         <v>37</v>
@@ -985,7 +988,7 @@
         <v>104</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
         <v>39</v>
@@ -1002,7 +1005,7 @@
         <v>105</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
         <v>43</v>
@@ -1019,7 +1022,7 @@
         <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
         <v>46</v>
@@ -1036,7 +1039,7 @@
         <v>107</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
         <v>48</v>
@@ -1053,7 +1056,7 @@
         <v>108</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -1070,7 +1073,7 @@
         <v>109</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -1087,7 +1090,7 @@
         <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -1104,7 +1107,7 @@
         <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
@@ -1121,7 +1124,7 @@
         <v>112</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -1138,7 +1141,7 @@
         <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
@@ -1155,7 +1158,7 @@
         <v>114</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
@@ -1172,7 +1175,7 @@
         <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
         <v>16</v>
@@ -1189,7 +1192,7 @@
         <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
@@ -1206,7 +1209,7 @@
         <v>117</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
@@ -1223,7 +1226,7 @@
         <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
         <v>20</v>
@@ -1240,7 +1243,7 @@
         <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
         <v>21</v>
@@ -1257,7 +1260,7 @@
         <v>120</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
         <v>25</v>
@@ -1274,7 +1277,7 @@
         <v>121</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C35" t="s">
         <v>27</v>
@@ -1291,7 +1294,7 @@
         <v>122</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C36" t="s">
         <v>28</v>
@@ -1308,7 +1311,7 @@
         <v>123</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C37" t="s">
         <v>29</v>
@@ -1325,7 +1328,7 @@
         <v>124</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C38" t="s">
         <v>31</v>
@@ -1342,7 +1345,7 @@
         <v>125</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C39" t="s">
         <v>32</v>
@@ -1359,7 +1362,7 @@
         <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C40" t="s">
         <v>33</v>
@@ -1376,7 +1379,7 @@
         <v>127</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C41" t="s">
         <v>34</v>
@@ -1393,7 +1396,7 @@
         <v>128</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
         <v>36</v>
@@ -1410,7 +1413,7 @@
         <v>129</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C43" t="s">
         <v>37</v>
@@ -1427,7 +1430,7 @@
         <v>130</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C44" t="s">
         <v>38</v>
@@ -1444,7 +1447,7 @@
         <v>131</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C45" t="s">
         <v>40</v>
@@ -1461,7 +1464,7 @@
         <v>132</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C46" t="s">
         <v>41</v>
@@ -1478,7 +1481,7 @@
         <v>133</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C47" t="s">
         <v>42</v>
@@ -1495,7 +1498,7 @@
         <v>134</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C48" t="s">
         <v>44</v>
@@ -1512,7 +1515,7 @@
         <v>135</v>
       </c>
       <c r="B49" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C49" t="s">
         <v>45</v>
@@ -1529,7 +1532,7 @@
         <v>136</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
         <v>47</v>
@@ -1546,7 +1549,7 @@
         <v>137</v>
       </c>
       <c r="B51" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C51" t="s">
         <v>48</v>

</xml_diff>